<commit_message>
double checked effects of slope change
</commit_message>
<xml_diff>
--- a/modflow_calibration/ss_calibration/slave_dir/manual_calib_results/manual_calib_results_summary.xlsx
+++ b/modflow_calibration/ss_calibration/slave_dir/manual_calib_results/manual_calib_results_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\projects\russian_river\model\RR_GSFLOW\modflow_calibration\ss_calibration\slave_dir\manual_calib_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C10B393-ACB9-47A8-8D8C-9D6F94B8DC3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B978210-FC22-46B2-91C9-06825D076B00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3435" yWindow="825" windowWidth="28845" windowHeight="13095" xr2:uid="{3A236F04-FC92-44B0-92B4-77ED56C436C9}"/>
+    <workbookView xWindow="6150" yWindow="1065" windowWidth="29295" windowHeight="17940" xr2:uid="{3A236F04-FC92-44B0-92B4-77ED56C436C9}"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -187,17 +187,17 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="9" tint="0.39997558519241921"/>
-      </bottom>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -225,7 +225,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A823FA12-B3FD-437C-A652-696C83E0F1FE}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:CN13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,7 +570,7 @@
     <col min="10" max="10" width="43.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:92" s="2" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -592,7 +602,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
@@ -620,7 +630,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -652,7 +662,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -684,7 +694,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
@@ -716,7 +726,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
@@ -748,67 +758,231 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:92" s="7" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="8">
         <v>5</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="5">
-        <v>1000</v>
-      </c>
-      <c r="E7" s="5">
-        <v>1</v>
-      </c>
-      <c r="F7" s="5">
-        <v>1000</v>
-      </c>
-      <c r="G7" s="5" t="s">
+      <c r="D7" s="9">
+        <v>1000</v>
+      </c>
+      <c r="E7" s="9">
+        <v>1</v>
+      </c>
+      <c r="F7" s="9">
+        <v>1000</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="4" t="s">
+      <c r="H7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="15" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="10"/>
+      <c r="AA7" s="10"/>
+      <c r="AB7" s="10"/>
+      <c r="AC7" s="10"/>
+      <c r="AD7" s="10"/>
+      <c r="AE7" s="10"/>
+      <c r="AF7" s="10"/>
+      <c r="AG7" s="10"/>
+      <c r="AH7" s="10"/>
+      <c r="AI7" s="10"/>
+      <c r="AJ7" s="10"/>
+      <c r="AK7" s="10"/>
+      <c r="AL7" s="10"/>
+      <c r="AM7" s="10"/>
+      <c r="AN7" s="10"/>
+      <c r="AO7" s="10"/>
+      <c r="AP7" s="10"/>
+      <c r="AQ7" s="10"/>
+      <c r="AR7" s="10"/>
+      <c r="AS7" s="10"/>
+      <c r="AT7" s="10"/>
+      <c r="AU7" s="10"/>
+      <c r="AV7" s="10"/>
+      <c r="AW7" s="10"/>
+      <c r="AX7" s="10"/>
+      <c r="AY7" s="10"/>
+      <c r="AZ7" s="10"/>
+      <c r="BA7" s="10"/>
+      <c r="BB7" s="10"/>
+      <c r="BC7" s="10"/>
+      <c r="BD7" s="10"/>
+      <c r="BE7" s="10"/>
+      <c r="BF7" s="10"/>
+      <c r="BG7" s="10"/>
+      <c r="BH7" s="10"/>
+      <c r="BI7" s="10"/>
+      <c r="BJ7" s="10"/>
+      <c r="BK7" s="10"/>
+      <c r="BL7" s="10"/>
+      <c r="BM7" s="10"/>
+      <c r="BN7" s="10"/>
+      <c r="BO7" s="10"/>
+      <c r="BP7" s="10"/>
+      <c r="BQ7" s="10"/>
+      <c r="BR7" s="10"/>
+      <c r="BS7" s="10"/>
+      <c r="BT7" s="10"/>
+      <c r="BU7" s="10"/>
+      <c r="BV7" s="10"/>
+      <c r="BW7" s="10"/>
+      <c r="BX7" s="10"/>
+      <c r="BY7" s="10"/>
+      <c r="BZ7" s="10"/>
+      <c r="CA7" s="10"/>
+      <c r="CB7" s="10"/>
+      <c r="CC7" s="10"/>
+      <c r="CD7" s="10"/>
+      <c r="CE7" s="10"/>
+      <c r="CF7" s="10"/>
+      <c r="CG7" s="10"/>
+      <c r="CH7" s="10"/>
+      <c r="CI7" s="10"/>
+      <c r="CJ7" s="10"/>
+      <c r="CK7" s="10"/>
+      <c r="CL7" s="10"/>
+      <c r="CM7" s="10"/>
+      <c r="CN7" s="10"/>
+    </row>
+    <row r="8" spans="1:92" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="11">
         <v>0</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="9">
-        <v>1</v>
-      </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9" t="s">
+      <c r="E8" s="12">
+        <v>1</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="9"/>
-      <c r="I8" s="8" t="s">
+      <c r="H8" s="12"/>
+      <c r="I8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13"/>
+      <c r="W8" s="13"/>
+      <c r="X8" s="13"/>
+      <c r="Y8" s="13"/>
+      <c r="Z8" s="13"/>
+      <c r="AA8" s="13"/>
+      <c r="AB8" s="13"/>
+      <c r="AC8" s="13"/>
+      <c r="AD8" s="13"/>
+      <c r="AE8" s="13"/>
+      <c r="AF8" s="13"/>
+      <c r="AG8" s="13"/>
+      <c r="AH8" s="13"/>
+      <c r="AI8" s="13"/>
+      <c r="AJ8" s="13"/>
+      <c r="AK8" s="13"/>
+      <c r="AL8" s="13"/>
+      <c r="AM8" s="13"/>
+      <c r="AN8" s="13"/>
+      <c r="AO8" s="13"/>
+      <c r="AP8" s="13"/>
+      <c r="AQ8" s="13"/>
+      <c r="AR8" s="13"/>
+      <c r="AS8" s="13"/>
+      <c r="AT8" s="13"/>
+      <c r="AU8" s="13"/>
+      <c r="AV8" s="13"/>
+      <c r="AW8" s="13"/>
+      <c r="AX8" s="13"/>
+      <c r="AY8" s="13"/>
+      <c r="AZ8" s="13"/>
+      <c r="BA8" s="13"/>
+      <c r="BB8" s="13"/>
+      <c r="BC8" s="13"/>
+      <c r="BD8" s="13"/>
+      <c r="BE8" s="13"/>
+      <c r="BF8" s="13"/>
+      <c r="BG8" s="13"/>
+      <c r="BH8" s="13"/>
+      <c r="BI8" s="13"/>
+      <c r="BJ8" s="13"/>
+      <c r="BK8" s="13"/>
+      <c r="BL8" s="13"/>
+      <c r="BM8" s="13"/>
+      <c r="BN8" s="13"/>
+      <c r="BO8" s="13"/>
+      <c r="BP8" s="13"/>
+      <c r="BQ8" s="13"/>
+      <c r="BR8" s="13"/>
+      <c r="BS8" s="13"/>
+      <c r="BT8" s="13"/>
+      <c r="BU8" s="13"/>
+      <c r="BV8" s="13"/>
+      <c r="BW8" s="13"/>
+      <c r="BX8" s="13"/>
+      <c r="BY8" s="13"/>
+      <c r="BZ8" s="13"/>
+      <c r="CA8" s="13"/>
+      <c r="CB8" s="13"/>
+      <c r="CC8" s="13"/>
+      <c r="CD8" s="13"/>
+      <c r="CE8" s="13"/>
+      <c r="CF8" s="13"/>
+      <c r="CG8" s="13"/>
+      <c r="CH8" s="13"/>
+      <c r="CI8" s="13"/>
+      <c r="CJ8" s="13"/>
+      <c r="CK8" s="13"/>
+      <c r="CL8" s="13"/>
+      <c r="CM8" s="13"/>
+      <c r="CN8" s="13"/>
+    </row>
+    <row r="9" spans="1:92" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
@@ -840,7 +1014,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:92" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>4</v>
       </c>
@@ -872,7 +1046,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:92" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>21</v>
       </c>
@@ -904,7 +1078,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:92" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>24</v>
       </c>
@@ -936,7 +1110,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:92" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>31</v>
       </c>
@@ -967,9 +1141,6 @@
       <c r="J13" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="3:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>